<commit_message>
Decision Tree.xlsx was updated to add a simple manager decision tree
</commit_message>
<xml_diff>
--- a/Documents/Decision Tree/Decision Tree.xlsx
+++ b/Documents/Decision Tree/Decision Tree.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="690" windowWidth="18675" windowHeight="11250" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="690" windowWidth="18675" windowHeight="11250" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Programmer(1)" sheetId="10" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="76">
   <si>
     <t>Value Measure</t>
   </si>
@@ -225,6 +225,30 @@
   <si>
     <t>Specifying</t>
   </si>
+  <si>
+    <t>Autonomy</t>
+  </si>
+  <si>
+    <t>Codification</t>
+  </si>
+  <si>
+    <t>Partial, check Focus Mode</t>
+  </si>
+  <si>
+    <t>Full Autonomy, determine Focus Mode by project's state</t>
+  </si>
+  <si>
+    <t>Analyst</t>
+  </si>
+  <si>
+    <t>Architect</t>
+  </si>
+  <si>
+    <t>Programmer</t>
+  </si>
+  <si>
+    <t>Aid, check which one will lend aid</t>
+  </si>
 </sst>
 </file>
 
@@ -18682,6 +18706,2286 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Root "/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="520700" y="857250"/>
+          <a:ext cx="88900" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TrNd "/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="762000"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Branch 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1019175" y="857250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Branch 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1019175" y="1619250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="TrNd 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2362200" y="762000"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Branch 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2771775" y="857250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Branch 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2771775" y="1619250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TrNd 11"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114800" y="762000"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Branch 111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="857250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Leaf 111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="785812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Branch 112"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="1619250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Leaf 112"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="1547812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Branch 113"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="2381250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Leaf 113"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="2309812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Branch 114"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="3143250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="44" name="Leaf 114"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="3071812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="45" name="FBranch 111"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4276725" y="857250"/>
+          <a:ext cx="247650" cy="1128712"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="FBranch 112"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4276725" y="1619250"/>
+          <a:ext cx="247650" cy="366712"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="47" name="FBranch 113"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4276725" y="1985962"/>
+          <a:ext cx="247650" cy="395288"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="FBranch 114"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4276725" y="1985962"/>
+          <a:ext cx="247650" cy="1157288"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="TrNd 12"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114800" y="3810000"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="59" name="Branch 121"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="3905250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="60" name="Leaf 121"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="3833812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="62" name="Branch 122"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="4667250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="63" name="Leaf 122"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="4595812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="65" name="Branch 123"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="5429250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Leaf 123"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="5357812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="75" name="Branch 124"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="6191250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="76" name="Leaf 124"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="6119812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="77" name="FBranch 121"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4276725" y="3905250"/>
+          <a:ext cx="247650" cy="1128712"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="FBranch 122"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4276725" y="4667250"/>
+          <a:ext cx="247650" cy="366712"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="FBranch 123"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4276725" y="5033962"/>
+          <a:ext cx="247650" cy="395288"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="FBranch 124"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4276725" y="5033962"/>
+          <a:ext cx="247650" cy="1157288"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="FBranch 11"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2524125" y="2000250"/>
+          <a:ext cx="247650" cy="1509712"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="82" name="FBranch 12"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2524125" y="3509962"/>
+          <a:ext cx="247650" cy="1538288"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="TrNd 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2362200" y="6858000"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="9999FF"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="89" name="Branch 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2771775" y="6953250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="90" name="Leaf 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="6881812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="92" name="Branch 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2771775" y="7715250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="93" name="Leaf 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="7643812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="94" name="XBranch 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114800" y="6953250"/>
+          <a:ext cx="1752600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="95" name="XBranch 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114800" y="7715250"/>
+          <a:ext cx="1752600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="97" name="Branch 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2771775" y="8477250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="98" name="Leaf 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="8405812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="99" name="FBranch 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2524125" y="6953250"/>
+          <a:ext cx="247650" cy="747712"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="100" name="FBranch 22"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2524125" y="7700962"/>
+          <a:ext cx="247650" cy="14288"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="101" name="FBranch 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2524125" y="7700962"/>
+          <a:ext cx="247650" cy="776288"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="102" name="FBranch 1"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="771525" y="3524250"/>
+          <a:ext cx="247650" cy="2081212"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="103" name="FBranch 2"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="771525" y="5605462"/>
+          <a:ext cx="247650" cy="2109788"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="104" name="XBranch 23"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4114800" y="8477250"/>
+          <a:ext cx="1752600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -22573,7 +24877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -23202,13 +25506,267 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="2.42578125" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" customWidth="1"/>
+    <col min="5" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="2.42578125" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="4.7109375" customWidth="1"/>
+    <col min="10" max="11" width="7.7109375" customWidth="1"/>
+    <col min="12" max="12" width="2.42578125" customWidth="1"/>
+    <col min="13" max="13" width="3.7109375" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" customWidth="1"/>
+    <col min="15" max="16" width="7.7109375" customWidth="1"/>
+    <col min="17" max="17" width="14.7109375" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="9:18">
+      <c r="Q1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="9:18">
+      <c r="N4" s="3" t="str">
+        <f>IF($K$12=$R$5,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="9:18">
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="9:18">
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="9:18">
+      <c r="N8" s="3" t="str">
+        <f>IF($K$12=$R$9,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="9:18">
+      <c r="Q9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="9:18">
+      <c r="I10" s="3" t="str">
+        <f>IF($F$20=$K$12,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="9:18">
+      <c r="K12">
+        <f>MAX($R$5,$R$9,$R$13,$R$17)</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="3" t="str">
+        <f>IF($K$12=$R$13,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="9:18">
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="9:18">
+      <c r="N16" s="3" t="str">
+        <f>IF($K$12=$R$17,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="Q17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="D18" s="3" t="str">
+        <f>IF($A$31=$F$20,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="Q19" s="2"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="F20">
+        <f>MAX($K$12,$K$28)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="3" t="str">
+        <f>IF($K$28=$R$21,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q20" s="2"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="Q21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="Q23" s="2"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="N24" s="3" t="str">
+        <f>IF($K$28=$R$25,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="Q25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="I26" s="3" t="str">
+        <f>IF($F$20=$K$28,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="K28">
+        <f>MAX($R$21,$R$25,$R$29,$R$33)</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="3" t="str">
+        <f>IF($K$28=$R$29,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="Q29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31">
+        <f>MAX($F$20,$F$42)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="N32" s="3" t="str">
+        <f>IF($K$28=$R$33,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="4:17">
+      <c r="Q33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:17">
+      <c r="I36" s="3" t="str">
+        <f>IF($F$42=$R$37,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="4:17">
+      <c r="Q37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="4:17">
+      <c r="Q39" s="2"/>
+    </row>
+    <row r="40" spans="4:17">
+      <c r="D40" s="3" t="str">
+        <f>IF($A$31=$F$42,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I40" s="3" t="str">
+        <f>IF($F$42=$R$41,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="4:17">
+      <c r="Q41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:17">
+      <c r="F42">
+        <f>MAX($R$37,$R$41,$R$45)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:17">
+      <c r="I44" s="3" t="str">
+        <f>IF($F$42=$R$45,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="4:17">
+      <c r="Q45" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated Decision Tree.xlsx Updated Raciocionio.docx Created the pptx for Raciocínio.docx Created the document for "Estudo Orientado" named Estudo_Orientado.docx (Draft for a paper)
</commit_message>
<xml_diff>
--- a/Documents/Decision Tree/Decision Tree.xlsx
+++ b/Documents/Decision Tree/Decision Tree.xlsx
@@ -6966,13 +6966,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7010,13 +7010,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7069,13 +7069,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7113,13 +7113,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7157,13 +7157,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7216,13 +7216,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7260,13 +7260,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7304,13 +7304,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7451,13 +7451,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7495,13 +7495,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7539,13 +7539,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7583,6 +7583,94 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Leaf 113"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5867400" y="2309812"/>
+          <a:ext cx="0" cy="142875"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Branch 114"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4524375" y="3143250"/>
+          <a:ext cx="1343025" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
@@ -7594,94 +7682,6 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="34" name="Leaf 113"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5867400" y="2309812"/>
-          <a:ext cx="0" cy="142875"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="43" name="Branch 114"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4524375" y="3143250"/>
-          <a:ext cx="1343025" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
         <xdr:cNvPr id="44" name="Leaf 114"/>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
@@ -7721,7 +7721,7 @@
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7759,13 +7759,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7803,13 +7803,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7847,13 +7847,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7891,13 +7891,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -7950,13 +7950,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -7994,13 +7994,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8038,13 +8038,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8082,13 +8082,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8126,13 +8126,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8170,13 +8170,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8214,13 +8214,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8258,13 +8258,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8302,13 +8302,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8346,13 +8346,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8390,13 +8390,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8434,13 +8434,13 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8478,13 +8478,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8522,13 +8522,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8566,13 +8566,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -8625,13 +8625,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8669,13 +8669,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8713,13 +8713,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8757,13 +8757,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8801,13 +8801,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8845,13 +8845,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8889,13 +8889,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8933,13 +8933,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>166687</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -8977,13 +8977,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9021,13 +9021,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9065,13 +9065,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9109,13 +9109,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9153,13 +9153,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9197,13 +9197,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -23828,7 +23828,7 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="Y38" sqref="Y38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -23849,7 +23849,7 @@
     <col min="18" max="18" width="3.7109375" customWidth="1"/>
     <col min="19" max="19" width="4.7109375" customWidth="1"/>
     <col min="20" max="21" width="7.7109375" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" customWidth="1"/>
+    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -24146,8 +24146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="Z39" sqref="Z39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24168,7 +24168,7 @@
     <col min="18" max="18" width="3.7109375" customWidth="1"/>
     <col min="19" max="19" width="4.7109375" customWidth="1"/>
     <col min="20" max="21" width="7.7109375" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" customWidth="1"/>
+    <col min="22" max="22" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -24466,10 +24466,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="W34" sqref="W34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24486,11 +24486,11 @@
     <col min="13" max="13" width="3.7109375" customWidth="1"/>
     <col min="14" max="14" width="4.7109375" customWidth="1"/>
     <col min="15" max="16" width="7.7109375" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" customWidth="1"/>
+    <col min="17" max="17" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="5:18">
+    <row r="1" spans="4:18">
       <c r="E1" s="19" t="s">
         <v>93</v>
       </c>
@@ -24501,228 +24501,215 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="5:18">
+    <row r="4" spans="4:18">
       <c r="N4" s="3" t="str">
-        <f>IF($K$12=$R$5,"&gt;&gt;&gt;","")</f>
+        <f>IF($K$10=$R$5,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="5:18">
+    <row r="5" spans="4:18">
       <c r="Q5" s="14" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="5:18">
-      <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="5:18">
-      <c r="N8" s="3" t="str">
-        <f>IF($K$12=$R$9,"&gt;&gt;&gt;","")</f>
+    <row r="6" spans="4:18">
+      <c r="N6" s="3" t="str">
+        <f>IF($K$10=$R$7,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="5:18">
-      <c r="Q9" s="14" t="s">
+    <row r="7" spans="4:18">
+      <c r="Q7" s="14" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="5:18">
-      <c r="I10" s="3" t="str">
-        <f>IF($F$20=$K$12,"&gt;&gt;&gt;","")</f>
+    <row r="8" spans="4:18">
+      <c r="I8" s="3" t="str">
+        <f>IF($F$16=$K$10,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="J10" s="18" t="s">
+      <c r="J8" s="18" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="5:18">
-      <c r="K12">
-        <f>MAX($R$5,$R$9,$R$13,$R$17)</f>
+    <row r="10" spans="4:18">
+      <c r="K10">
+        <f>MAX($R$5,$R$7,$R$11,$R$13)</f>
         <v>0</v>
       </c>
+      <c r="N10" s="3" t="str">
+        <f>IF($K$10=$R$11,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="4:18">
+      <c r="Q11" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="4:18">
       <c r="N12" s="3" t="str">
-        <f>IF($K$12=$R$13,"&gt;&gt;&gt;","")</f>
+        <f>IF($K$10=$R$13,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="5:18">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="4:18">
       <c r="Q13" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="5:18">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="4:18">
+      <c r="D14" s="3" t="str">
+        <f>IF($A$25=$F$16,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="4:18">
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="4:18">
+      <c r="F16">
+        <f>MAX($K$10,$K$22)</f>
+        <v>0</v>
+      </c>
       <c r="N16" s="3" t="str">
-        <f>IF($K$12=$R$17,"&gt;&gt;&gt;","")</f>
+        <f>IF($K$22=$R$17,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O16" s="3" t="s">
-        <v>81</v>
-      </c>
+      <c r="O16" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q16" s="2"/>
     </row>
     <row r="17" spans="1:17">
       <c r="Q17" s="14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="N18" s="3" t="str">
+        <f>IF($K$22=$R$19,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O18" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="Q19" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="I20" s="3" t="str">
+        <f>IF($F$16=$K$22,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="J20" s="18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="K22">
+        <f>MAX($R$17,$R$19,$R$23,$R$26)</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="3" t="str">
+        <f>IF($K$22=$R$23,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O22" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="Q23" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25">
+        <f>MAX($F$16,$F$31)</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="3" t="str">
+        <f>IF($K$22=$R$26,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="O25" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="Q26" s="14" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
-      <c r="D18" s="3" t="str">
-        <f>IF($A$31=$F$20,"&gt;&gt;&gt;","")</f>
+    <row r="27" spans="1:17">
+      <c r="I27" s="3" t="str">
+        <f>IF($F$31=$R$28,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17">
-      <c r="Q19" s="2"/>
-    </row>
-    <row r="20" spans="1:17">
-      <c r="F20">
-        <f>MAX($K$12,$K$28)</f>
+      <c r="J27" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="Q28" s="14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="D29" s="3" t="str">
+        <f>IF($A$25=$F$31,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" s="3" t="str">
+        <f>IF($F$31=$R$30,"&gt;&gt;&gt;","")</f>
+        <v>&gt;&gt;&gt;</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="Q30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="F31">
+        <f>MAX($R$28,$R$30,$R$32)</f>
         <v>0</v>
       </c>
-      <c r="N20" s="3" t="str">
-        <f>IF($K$28=$R$21,"&gt;&gt;&gt;","")</f>
+      <c r="I31" s="3" t="str">
+        <f>IF($F$31=$R$32,"&gt;&gt;&gt;","")</f>
         <v>&gt;&gt;&gt;</v>
       </c>
-      <c r="O20" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q20" s="2"/>
-    </row>
-    <row r="21" spans="1:17">
-      <c r="Q21" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17">
-      <c r="Q23" s="2"/>
-    </row>
-    <row r="24" spans="1:17">
-      <c r="N24" s="3" t="str">
-        <f>IF($K$28=$R$25,"&gt;&gt;&gt;","")</f>
-        <v>&gt;&gt;&gt;</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17">
-      <c r="Q25" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17">
-      <c r="I26" s="3" t="str">
-        <f>IF($F$20=$K$28,"&gt;&gt;&gt;","")</f>
-        <v>&gt;&gt;&gt;</v>
-      </c>
-      <c r="J26" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="K28">
-        <f>MAX($R$21,$R$25,$R$29,$R$33)</f>
-        <v>0</v>
-      </c>
-      <c r="N28" s="3" t="str">
-        <f>IF($K$28=$R$29,"&gt;&gt;&gt;","")</f>
-        <v>&gt;&gt;&gt;</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="Q29" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17">
-      <c r="A31">
-        <f>MAX($F$20,$F$42)</f>
-        <v>0</v>
+      <c r="J31" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:17">
-      <c r="N32" s="3" t="str">
-        <f>IF($K$28=$R$33,"&gt;&gt;&gt;","")</f>
-        <v>&gt;&gt;&gt;</v>
-      </c>
-      <c r="O32" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="4:17">
-      <c r="Q33" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="36" spans="4:17">
-      <c r="I36" s="3" t="str">
-        <f>IF($F$42=$R$37,"&gt;&gt;&gt;","")</f>
-        <v>&gt;&gt;&gt;</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="4:17">
-      <c r="Q37" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="4:17">
-      <c r="Q39" s="2"/>
-    </row>
-    <row r="40" spans="4:17">
-      <c r="D40" s="3" t="str">
-        <f>IF($A$31=$F$42,"&gt;&gt;&gt;","")</f>
-        <v>&gt;&gt;&gt;</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="I40" s="3" t="str">
-        <f>IF($F$42=$R$41,"&gt;&gt;&gt;","")</f>
-        <v>&gt;&gt;&gt;</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="4:17">
-      <c r="Q41" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="4:17">
-      <c r="F42">
-        <f>MAX($R$37,$R$41,$R$45)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="4:17">
-      <c r="I44" s="3" t="str">
-        <f>IF($F$42=$R$45,"&gt;&gt;&gt;","")</f>
-        <v>&gt;&gt;&gt;</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="4:17">
-      <c r="Q45" s="14" t="s">
+      <c r="Q32" s="14" t="s">
         <v>76</v>
       </c>
     </row>
@@ -24811,8 +24798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AK91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>